<commit_message>
feat: new flag TCS_EVALUATION!
New flag that allows the user to decide if the current sharing temperature should be evaluated at each time steps or if it should be evaluated only at the beginning or at the end of the simulation.

This is a very rough solution and should be impoved as soon as possible.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_1_operation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniele.Placido\OneDrive - Politecnico di Torino\OPENSC2\Description_of_Components\input_file_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B300486-29C0-4BD6-A652-17A335E60A05}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="720" yWindow="720" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="92">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>Professor L. Savoldi NEEDS to fullfill this values</t>
+  </si>
+  <si>
+    <t>TCS_EVALUATION</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>Flag to decide if the current sharing temperature should be evaluated at each time steps or not (improve speed). Possible values: False = evaluate the current sharing temperature only at the initialization and at the end of the simulation; True = evaluate the current sharing temperature at each time steps (affects computaion time). Defaults to False.</t>
   </si>
 </sst>
 </file>
@@ -570,75 +579,6 @@
           <cell r="A1" t="str">
             <v>CHAN</v>
           </cell>
-          <cell r="E1">
-            <v>1</v>
-          </cell>
-          <cell r="F1">
-            <v>2</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>STR_MIX</v>
-          </cell>
-          <cell r="E1">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>STR_SC</v>
-          </cell>
-          <cell r="E1">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>STR_STAB</v>
-          </cell>
-          <cell r="E1">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>Z_JACKET</v>
-          </cell>
-          <cell r="E1">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="CHAN"/>
-      <sheetName val="STR_MIX"/>
-      <sheetName val="STR_SC"/>
-      <sheetName val="STR_STAB"/>
-      <sheetName val="Z_JACKET"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>CHAN</v>
-          </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
@@ -680,6 +620,60 @@
         <row r="1">
           <cell r="A1" t="str">
             <v>Z_JACKET</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="CHAN"/>
+      <sheetName val="STR_MIX"/>
+      <sheetName val="STR_SC"/>
+      <sheetName val="STR_STAB"/>
+      <sheetName val="Z_JACKET"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="E1">
+            <v>1</v>
+          </cell>
+          <cell r="F1">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="E1">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2">
+        <row r="1">
+          <cell r="E1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3">
+        <row r="1">
+          <cell r="E1">
+            <v>0</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="1">
+          <cell r="E1">
+            <v>1</v>
           </cell>
         </row>
       </sheetData>
@@ -1006,7 +1000,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="str">
-        <f>[2]CHAN!$A$1</f>
+        <f>[1]CHAN!$A$1</f>
         <v>CHAN</v>
       </c>
       <c r="B1" s="19">
@@ -1018,11 +1012,11 @@
         <v>42</v>
       </c>
       <c r="E1" s="18">
-        <f>[1]CHAN!E$1</f>
+        <f>[2]CHAN!E$1</f>
         <v>1</v>
       </c>
       <c r="F1" s="18">
-        <f>[1]CHAN!F$1</f>
+        <f>[2]CHAN!F$1</f>
         <v>2</v>
       </c>
     </row>
@@ -1044,19 +1038,19 @@
     </row>
     <row r="3" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="21" t="str">
-        <f>[2]CHAN!A$3</f>
+        <f>[1]CHAN!A$3</f>
         <v>Variable name</v>
       </c>
       <c r="B3" s="21" t="str">
-        <f>[2]CHAN!B$3</f>
+        <f>[1]CHAN!B$3</f>
         <v>Unit</v>
       </c>
       <c r="C3" s="21" t="str">
-        <f>[2]CHAN!C$3</f>
+        <f>[1]CHAN!C$3</f>
         <v>Variable type</v>
       </c>
       <c r="D3" s="21" t="str">
-        <f>[2]CHAN!D$3</f>
+        <f>[1]CHAN!D$3</f>
         <v>Note/comments</v>
       </c>
       <c r="E3" s="18" t="str">
@@ -1261,16 +1255,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26:E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.453125" style="25" customWidth="1"/>
@@ -1280,7 +1274,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="str">
-        <f>[2]STR_MIX!$A$1</f>
+        <f>[1]STR_MIX!$A$1</f>
         <v>STR_MIX</v>
       </c>
       <c r="B1" s="22">
@@ -1292,7 +1286,7 @@
         <v>44</v>
       </c>
       <c r="E1" s="18">
-        <f>[1]STR_MIX!E$1</f>
+        <f>[2]STR_MIX!E$1</f>
         <v>1</v>
       </c>
     </row>
@@ -1702,7 +1696,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="10.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1712,19 +1722,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04312A78-FBC2-476F-A763-194D3CD2A19F}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6328125" style="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="69.453125" style="25" customWidth="1"/>
@@ -1734,7 +1744,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="str">
-        <f>[2]STR_SC!$A$1</f>
+        <f>[1]STR_SC!$A$1</f>
         <v>STR_SC</v>
       </c>
       <c r="B1" s="22">
@@ -1746,7 +1756,7 @@
         <v>57</v>
       </c>
       <c r="E1" s="18">
-        <f>[1]STR_STAB!E$1</f>
+        <f>[2]STR_STAB!E$1</f>
         <v>0</v>
       </c>
     </row>
@@ -2153,6 +2163,23 @@
         <v>75</v>
       </c>
       <c r="E25" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2186,7 +2213,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="str">
-        <f>[2]STR_STAB!$A$1</f>
+        <f>[1]STR_STAB!$A$1</f>
         <v>STR_STAB</v>
       </c>
       <c r="B1" s="22">
@@ -2198,7 +2225,7 @@
         <v>58</v>
       </c>
       <c r="E1" s="18">
-        <f>[1]STR_SC!E$1</f>
+        <f>[2]STR_SC!E$1</f>
         <v>0</v>
       </c>
     </row>
@@ -2583,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
@@ -2603,7 +2630,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="str">
-        <f>[2]Z_JACKET!$A$1</f>
+        <f>[1]Z_JACKET!$A$1</f>
         <v>Z_JACKET</v>
       </c>
       <c r="B1" s="22">
@@ -2615,7 +2642,7 @@
         <v>59</v>
       </c>
       <c r="E1" s="18">
-        <f>[1]Z_JACKET!E$1</f>
+        <f>[2]Z_JACKET!E$1</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: change not used input file to none.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_1_operation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EA9CCD4-707F-4DD8-8155-A1828DE645E4}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9CBC064-7B74-47F4-B3FC-E89FCD361EC9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -283,9 +283,6 @@
     <t>FLOWDIR</t>
   </si>
   <si>
-    <t>backward</t>
-  </si>
-  <si>
     <t>flag to define the flow direction. Possible values: forward or Forward or FORWARD (inlet at x  = 0 and outlet at x = L); backward or Backward or BACKWARD (inlet at x = L and outlet at x = 0). Defaults to forward. If chanels are in hydraulic parallel, they must all have the same flow direction.</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>Flag to specify the kind of interpolator for the heat data, if IQFUN = -1. Possible values: linear = liear interpolation; cubic = use spline function of third order.</t>
+  </si>
+  <si>
+    <t>forward</t>
   </si>
 </sst>
 </file>
@@ -951,7 +951,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1201,13 +1201,13 @@
         <v>77</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1221,11 +1221,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
+      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1309,7 +1309,7 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>28</v>
@@ -1318,10 +1318,10 @@
         <v>77</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1335,7 +1335,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="25">
         <v>0</v>
@@ -1343,7 +1343,7 @@
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>28</v>
@@ -1352,10 +1352,10 @@
         <v>77</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1386,7 +1386,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="24">
         <v>1</v>
@@ -1403,7 +1403,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="24">
         <v>1</v>
@@ -1473,7 +1473,7 @@
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>28</v>
@@ -1482,10 +1482,10 @@
         <v>77</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1507,7 +1507,7 @@
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>28</v>
@@ -1516,10 +1516,10 @@
         <v>77</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1550,7 +1550,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" s="24">
         <v>1</v>
@@ -1558,7 +1558,7 @@
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>28</v>
@@ -1567,10 +1567,10 @@
         <v>77</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1587,7 +1587,7 @@
         <v>47</v>
       </c>
       <c r="E21" s="24">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1604,7 +1604,7 @@
         <v>48</v>
       </c>
       <c r="E22" s="24">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1728,16 +1728,16 @@
     </row>
     <row r="30" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="D30" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="E30" s="24" t="b">
         <v>0</v>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>28</v>
@@ -1852,10 +1852,10 @@
         <v>77</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1869,7 +1869,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="25">
         <v>0</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>28</v>
@@ -1886,10 +1886,10 @@
         <v>77</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -1920,7 +1920,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="24">
         <v>1</v>
@@ -1937,7 +1937,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="24">
         <v>1</v>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>28</v>
@@ -2016,10 +2016,10 @@
         <v>77</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2041,7 +2041,7 @@
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>28</v>
@@ -2050,10 +2050,10 @@
         <v>77</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2084,7 +2084,7 @@
         <v>26</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E19" s="24">
         <v>0</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>28</v>
@@ -2101,10 +2101,10 @@
         <v>77</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -2262,16 +2262,16 @@
     </row>
     <row r="30" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="D30" s="20" t="s">
         <v>83</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>84</v>
       </c>
       <c r="E30" s="24" t="b">
         <v>0</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>28</v>
@@ -2385,10 +2385,10 @@
         <v>77</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2402,7 +2402,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="25">
         <v>0</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>28</v>
@@ -2419,10 +2419,10 @@
         <v>77</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2453,7 +2453,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -2470,7 +2470,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="24">
         <v>0</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>28</v>
@@ -2549,10 +2549,10 @@
         <v>77</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2566,7 +2566,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="24">
         <v>0</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>28</v>
@@ -2583,10 +2583,10 @@
         <v>77</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2753,8 +2753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>28</v>
@@ -2851,10 +2851,10 @@
         <v>77</v>
       </c>
       <c r="D5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E5" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -2868,7 +2868,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E6" s="25">
         <v>0</v>
@@ -2876,7 +2876,7 @@
     </row>
     <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>28</v>
@@ -2885,10 +2885,10 @@
         <v>77</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="24" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="24" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -2919,7 +2919,7 @@
         <v>27</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E9" s="24">
         <v>0</v>
@@ -2936,7 +2936,7 @@
         <v>27</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E10" s="24">
         <v>0</v>
@@ -3006,7 +3006,7 @@
     </row>
     <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B15" s="24" t="s">
         <v>28</v>
@@ -3015,10 +3015,10 @@
         <v>77</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -3032,7 +3032,7 @@
         <v>26</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E16" s="24">
         <v>0</v>
@@ -3040,7 +3040,7 @@
     </row>
     <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" s="24" t="s">
         <v>28</v>
@@ -3049,10 +3049,10 @@
         <v>77</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E17" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
feat!: update sheets in file conductor_operation.
New variables in sheets STR_MIX, STR_SC and STR_STAB to deal with electric module input:
    * FIX_POTENTIAL_FLAG
    * FIX_POTENTIAL_NUMBER
    * FIX_POTENTIAL_COORDINATE
    * FIX_POTENTIAL_VALUE
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_1_operation.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_1_operation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9CBC064-7B74-47F4-B3FC-E89FCD361EC9}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{6F6F60DD-9A76-4126-9A28-D0FBB56FD81E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA1F6644-7BFB-44AA-81D5-D419D8C9AEB5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CHAN" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="108">
   <si>
     <t>IBIFUN</t>
   </si>
@@ -338,6 +338,33 @@
   </si>
   <si>
     <t>forward</t>
+  </si>
+  <si>
+    <t>FIX_POTENTIAL_FLAG</t>
+  </si>
+  <si>
+    <t>Flag to allow user to specify the potential value in some axial location of the conductor. Possible values: 1 = user can assign the position and the value of the potential; 0 = user can not assign these values. Defaults to 0</t>
+  </si>
+  <si>
+    <t>FIX_POTENTIAL_NUMBER</t>
+  </si>
+  <si>
+    <t>The number of potential values to be assigned, if FIX_POTENTIAL_FLAG is True.</t>
+  </si>
+  <si>
+    <t>FIX_POTENTIAL_COORDINATE</t>
+  </si>
+  <si>
+    <t>List of axial coordinate at which assing the fix potential value, separated by a comma, if FIX_POTENTIAL_FLAG is True. Ex, if at z = 0.5m z = 1.0m and z = 1.5m user wants to fix the potential value, write 0.5,1.0,1.5.</t>
+  </si>
+  <si>
+    <t>FIX_POTENTIAL_VALUE</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>List of fix potential value the user wants to assig, separated by a comma, if FIX_POTENTIAL_FLAG is True. Ex, if user wants to assign three potential values, write: 0.0,2.0,4.0.</t>
   </si>
 </sst>
 </file>
@@ -406,7 +433,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -510,6 +537,10 @@
     </xf>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -954,17 +985,17 @@
       <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.08984375" style="4" customWidth="1"/>
-    <col min="5" max="6" width="17.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.90625" style="5"/>
+    <col min="1" max="1" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="62.140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>[1]CHAN!$A$1</f>
         <v>CHAN</v>
@@ -986,7 +1017,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="6"/>
@@ -1002,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="str">
         <f>[1]CHAN!A$3</f>
         <v>Variable name</v>
@@ -1028,7 +1059,7 @@
         <v>CHAN_2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1099,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1088,7 +1119,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
@@ -1108,7 +1139,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -1128,7 +1159,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1148,7 +1179,7 @@
         <v>590000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>29</v>
       </c>
@@ -1170,7 +1201,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>19</v>
       </c>
@@ -1190,7 +1221,7 @@
         <v>1.248E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>79</v>
       </c>
@@ -1219,32 +1250,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E23" sqref="E23"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="15.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]STR_MIX!$A$1</f>
         <v>STR_MIX</v>
       </c>
       <c r="B1" s="17">
-        <f>SUM(E2:AE2)</f>
+        <f>SUM(E2:Z2)</f>
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
@@ -1256,7 +1287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1268,7 +1299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1290,7 +1321,7 @@
         <v>STR_MIX_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -1307,7 +1338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>84</v>
       </c>
@@ -1324,9 +1355,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>0</v>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>28</v>
@@ -1335,411 +1366,479 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="E10" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="B11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D11" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E11" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="B12" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D12" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="E12" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="20" t="s">
+      <c r="B14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="E14" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="B15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="B16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="B17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="B18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E19" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="E20" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E21" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="20" t="s">
+      <c r="B22" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B23" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="E23" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="24" t="s">
+      <c r="B24" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E24" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B25" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="C25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="E25" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B26" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="20" t="s">
+      <c r="C26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E26" s="24">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B27" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="20" t="s">
+      <c r="C27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E27" s="24">
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B28" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="C28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E28" s="24">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="C29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E29" s="24">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="B30" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="E30" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="B31" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B32" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="20" t="s">
+      <c r="C32" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E28" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+      <c r="E32" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B33" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="20" t="s">
+      <c r="C33" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="E33" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="B34" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D34" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="24" t="b">
+      <c r="E34" s="24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -1752,27 +1851,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04312A78-FBC2-476F-A763-194D3CD2A19F}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D10" sqref="D10"/>
       <selection pane="topRight" activeCell="D10" sqref="D10"/>
       <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD30"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6328125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="20" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]STR_SC!$A$1</f>
         <v>STR_SC</v>
@@ -1790,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1802,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -1824,7 +1923,7 @@
         <v>STR_SC_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -1841,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>84</v>
       </c>
@@ -1858,9 +1957,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>0</v>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>28</v>
@@ -1869,411 +1968,479 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="E10" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="B11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D11" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E11" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="B12" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D12" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="E12" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="E13" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="20" t="s">
+      <c r="B14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="E14" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="B15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="B16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="B17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="B18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E19" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="E20" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E21" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="20" t="s">
+      <c r="B22" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="E22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="B23" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D23" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="E23" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B20" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="24" t="s">
+      <c r="B24" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D24" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E24" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B25" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="20" t="s">
+      <c r="C25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B26" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="20" t="s">
+      <c r="C26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B27" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="20" t="s">
+      <c r="C27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B28" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="20" t="s">
+      <c r="C28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="E28" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="C29" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+      <c r="E29" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="B30" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+      <c r="E30" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="24" t="s">
+      <c r="B31" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D31" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="15" t="s">
+      <c r="E31" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B32" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="20" t="s">
+      <c r="C32" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="15" t="s">
+      <c r="E32" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="24" t="s">
+      <c r="B33" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="20" t="s">
+      <c r="C33" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="15" t="s">
+      <c r="E33" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="24" t="s">
+      <c r="B34" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D34" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="24" t="b">
+      <c r="E34" s="24" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2285,27 +2452,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791C09E2-9ECD-4150-8BC7-6143A0B898FB}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D22" sqref="D22"/>
       <selection pane="topRight" activeCell="D22" sqref="D22"/>
       <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD26"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="5"/>
+    <col min="1" max="1" width="27.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]STR_STAB!$A$1</f>
         <v>STR_STAB</v>
@@ -2323,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2335,7 +2502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -2357,7 +2524,7 @@
         <v>STR_STAB_0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -2374,7 +2541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>84</v>
       </c>
@@ -2391,9 +2558,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>0</v>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="s">
+        <v>99</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>28</v>
@@ -2402,343 +2569,411 @@
         <v>26</v>
       </c>
       <c r="D6" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="E6" s="25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="E10" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="24" t="s">
+      <c r="B11" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D11" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E11" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="24" t="s">
+      <c r="B12" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D12" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="E12" s="25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="20" t="s">
+      <c r="B13" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="E13" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="20" t="s">
+      <c r="B14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
+      <c r="E14" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
+      <c r="B15" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="19" t="s">
+      <c r="B16" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+      <c r="B17" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="B18" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D18" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+      <c r="E18" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="24" t="s">
+      <c r="B19" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E19" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="24" t="s">
+      <c r="B20" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D20" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
+      <c r="E20" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B17" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="24" t="s">
+      <c r="B21" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D21" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E21" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B22" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="4" t="s">
+      <c r="C22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+      <c r="E22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B23" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="20" t="s">
+      <c r="C23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="E23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B24" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="4" t="s">
+      <c r="C24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+      <c r="E24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B25" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="4" t="s">
+      <c r="C25" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="15" t="s">
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B26" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="C26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="4" t="s">
+      <c r="B27" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B24" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="24" t="s">
+      <c r="B28" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D28" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="15" t="s">
+      <c r="E28" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B29" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="20" t="s">
+      <c r="C29" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+      <c r="E29" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="C30" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="27">
+      <c r="E30" s="27">
         <v>0</v>
       </c>
     </row>
@@ -2761,17 +2996,17 @@
       <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.453125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.90625" style="5"/>
+    <col min="1" max="1" width="14.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="str">
         <f>[1]Z_JACKET!$A$1</f>
         <v>Z_JACKET</v>
@@ -2789,7 +3024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2801,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="str">
         <f>CHAN!A3</f>
         <v>Variable name</v>
@@ -2823,7 +3058,7 @@
         <v>Z_JACKET_1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>6</v>
       </c>
@@ -2840,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>84</v>
       </c>
@@ -2857,7 +3092,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>0</v>
       </c>
@@ -2874,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>88</v>
       </c>
@@ -2891,7 +3126,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>76</v>
       </c>
@@ -2908,7 +3143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>20</v>
       </c>
@@ -2925,7 +3160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>21</v>
       </c>
@@ -2942,7 +3177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>22</v>
       </c>
@@ -2957,7 +3192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>23</v>
       </c>
@@ -2972,7 +3207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>24</v>
       </c>
@@ -2987,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>2</v>
       </c>
@@ -3004,7 +3239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>91</v>
       </c>
@@ -3021,7 +3256,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>35</v>
       </c>
@@ -3038,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>96</v>
       </c>
@@ -3055,7 +3290,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>36</v>
       </c>
@@ -3072,7 +3307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>37</v>
       </c>
@@ -3089,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>5</v>
       </c>
@@ -3106,7 +3341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
         <v>38</v>
       </c>
@@ -3123,7 +3358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
         <v>39</v>
       </c>
@@ -3140,7 +3375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>10</v>
       </c>
@@ -3157,7 +3392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>11</v>
       </c>
@@ -3174,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
         <v>12</v>
       </c>

</xml_diff>